<commit_message>
fixed arguments in krispmer run
</commit_message>
<xml_diff>
--- a/expt03/mouse/chr1-tgt1.xlsx
+++ b/expt03/mouse/chr1-tgt1.xlsx
@@ -1,13 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbr5797/krispmer/krispmer-expreminets/expt03/mouse/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1183A2BB-CE36-B445-A6E4-4358AFD58FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="gRNAs" r:id="rId3" sheetId="1"/>
+    <sheet name="gRNAs" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1493,11 +1513,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1509,7 +1528,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -1527,18 +1546,333 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="217" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1579,7 +1913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1595,20 +1929,20 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="n">
-        <v>4.0</v>
+      <c r="F2">
+        <v>4</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>0.45274999737739563</v>
       </c>
-      <c r="I2" t="n">
-        <v>0.9463030099868774</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1.0</v>
+      <c r="I2">
+        <v>0.94630300998687744</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>19</v>
@@ -1620,7 +1954,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1636,20 +1970,20 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="n">
-        <v>4.0</v>
+      <c r="F3">
+        <v>4</v>
       </c>
       <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="n">
-        <v>0.5011969804763794</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.6462910175323486</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2.0</v>
+      <c r="H3">
+        <v>0.50119698047637939</v>
+      </c>
+      <c r="I3">
+        <v>0.64629101753234863</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
       </c>
       <c r="K3" t="s">
         <v>24</v>
@@ -1661,7 +1995,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1677,20 +2011,20 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="n">
-        <v>8.0</v>
+      <c r="F4">
+        <v>8</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="H4" t="n">
-        <v>0.610713005065918</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.5050129890441895</v>
-      </c>
-      <c r="J4" t="n">
-        <v>3.0</v>
+      <c r="H4">
+        <v>0.61071300506591797</v>
+      </c>
+      <c r="I4">
+        <v>0.50501298904418945</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
       </c>
       <c r="K4" t="s">
         <v>30</v>
@@ -1702,7 +2036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1718,20 +2052,20 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="n">
-        <v>9.0</v>
+      <c r="F5">
+        <v>9</v>
       </c>
       <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="n">
-        <v>0.6165800094604492</v>
-      </c>
-      <c r="I5" t="n">
+      <c r="H5">
+        <v>0.61658000946044922</v>
+      </c>
+      <c r="I5">
         <v>0.38544100522994995</v>
       </c>
-      <c r="J5" t="n">
-        <v>4.0</v>
+      <c r="J5">
+        <v>4</v>
       </c>
       <c r="K5" t="s">
         <v>35</v>
@@ -1743,7 +2077,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1759,20 +2093,20 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="n">
-        <v>9.0</v>
+      <c r="F6">
+        <v>9</v>
       </c>
       <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>0.35620200634002686</v>
       </c>
-      <c r="I6" t="n">
-        <v>0.3638690114021301</v>
-      </c>
-      <c r="J6" t="n">
-        <v>5.0</v>
+      <c r="I6">
+        <v>0.36386901140213013</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
       </c>
       <c r="K6" t="s">
         <v>39</v>
@@ -1784,7 +2118,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1800,20 +2134,20 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="n">
-        <v>11.0</v>
+      <c r="F7">
+        <v>11</v>
       </c>
       <c r="G7" t="s">
         <v>42</v>
       </c>
-      <c r="H7" t="n">
-        <v>0.3270510137081146</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.7733150124549866</v>
-      </c>
-      <c r="J7" t="n">
-        <v>6.0</v>
+      <c r="H7">
+        <v>0.32705101370811462</v>
+      </c>
+      <c r="I7">
+        <v>0.77331501245498657</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
       </c>
       <c r="K7" t="s">
         <v>43</v>
@@ -1825,7 +2159,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1841,20 +2175,20 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" t="n">
-        <v>11.0</v>
+      <c r="F8">
+        <v>11</v>
       </c>
       <c r="G8" t="s">
         <v>46</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>0.36333900690078735</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8">
         <v>0.38765498995780945</v>
       </c>
-      <c r="J8" t="n">
-        <v>7.0</v>
+      <c r="J8">
+        <v>7</v>
       </c>
       <c r="K8" t="s">
         <v>47</v>
@@ -1866,7 +2200,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1882,20 +2216,20 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="n">
-        <v>11.0</v>
+      <c r="F9">
+        <v>11</v>
       </c>
       <c r="G9" t="s">
         <v>46</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>0.5462610125541687</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9">
         <v>0.40845999121665955</v>
       </c>
-      <c r="J9" t="n">
-        <v>8.0</v>
+      <c r="J9">
+        <v>8</v>
       </c>
       <c r="K9" t="s">
         <v>51</v>
@@ -1907,7 +2241,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1923,20 +2257,20 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="n">
-        <v>11.0</v>
+      <c r="F10">
+        <v>11</v>
       </c>
       <c r="G10" t="s">
         <v>46</v>
       </c>
-      <c r="H10" t="n">
-        <v>0.5998110175132751</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.7356070280075073</v>
-      </c>
-      <c r="J10" t="n">
-        <v>9.0</v>
+      <c r="H10">
+        <v>0.59981101751327515</v>
+      </c>
+      <c r="I10">
+        <v>0.73560702800750732</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
       </c>
       <c r="K10" t="s">
         <v>55</v>
@@ -1948,7 +2282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1964,20 +2298,20 @@
       <c r="E11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="n">
-        <v>13.0</v>
+      <c r="F11">
+        <v>13</v>
       </c>
       <c r="G11" t="s">
         <v>59</v>
       </c>
-      <c r="H11" t="n">
-        <v>0.5274419784545898</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.4016779959201813</v>
-      </c>
-      <c r="J11" t="n">
-        <v>10.0</v>
+      <c r="H11">
+        <v>0.52744197845458984</v>
+      </c>
+      <c r="I11">
+        <v>0.40167799592018127</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
       </c>
       <c r="K11" t="s">
         <v>60</v>
@@ -1989,7 +2323,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2005,20 +2339,20 @@
       <c r="E12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" t="n">
-        <v>14.0</v>
+      <c r="F12">
+        <v>14</v>
       </c>
       <c r="G12" t="s">
         <v>64</v>
       </c>
-      <c r="H12" t="n">
-        <v>0.4581649899482727</v>
-      </c>
-      <c r="I12" t="n">
+      <c r="H12">
+        <v>0.45816498994827271</v>
+      </c>
+      <c r="I12">
         <v>0.30589398741722107</v>
       </c>
-      <c r="J12" t="n">
-        <v>11.0</v>
+      <c r="J12">
+        <v>11</v>
       </c>
       <c r="K12" t="s">
         <v>65</v>
@@ -2030,7 +2364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2046,20 +2380,20 @@
       <c r="E13" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="n">
-        <v>14.0</v>
+      <c r="F13">
+        <v>14</v>
       </c>
       <c r="G13" t="s">
         <v>64</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13">
         <v>0.5531650185585022</v>
       </c>
-      <c r="I13" t="n">
-        <v>0.3583270013332367</v>
-      </c>
-      <c r="J13" t="n">
-        <v>12.0</v>
+      <c r="I13">
+        <v>0.35832700133323669</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
       </c>
       <c r="K13" t="s">
         <v>69</v>
@@ -2071,7 +2405,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2087,20 +2421,20 @@
       <c r="E14" t="s">
         <v>17</v>
       </c>
-      <c r="F14" t="n">
-        <v>15.0</v>
+      <c r="F14">
+        <v>15</v>
       </c>
       <c r="G14" t="s">
         <v>72</v>
       </c>
-      <c r="H14" t="n">
-        <v>0.6039360165596008</v>
-      </c>
-      <c r="I14" t="n">
+      <c r="H14">
+        <v>0.60393601655960083</v>
+      </c>
+      <c r="I14">
         <v>0.21500399708747864</v>
       </c>
-      <c r="J14" t="n">
-        <v>13.0</v>
+      <c r="J14">
+        <v>13</v>
       </c>
       <c r="K14" t="s">
         <v>73</v>
@@ -2112,7 +2446,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2128,20 +2462,20 @@
       <c r="E15" t="s">
         <v>17</v>
       </c>
-      <c r="F15" t="n">
-        <v>15.0</v>
+      <c r="F15">
+        <v>15</v>
       </c>
       <c r="G15" t="s">
         <v>72</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15">
         <v>0.45570799708366394</v>
       </c>
-      <c r="I15" t="n">
-        <v>0.2547900080680847</v>
-      </c>
-      <c r="J15" t="n">
-        <v>14.0</v>
+      <c r="I15">
+        <v>0.25479000806808472</v>
+      </c>
+      <c r="J15">
+        <v>14</v>
       </c>
       <c r="K15" t="s">
         <v>77</v>
@@ -2153,7 +2487,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2169,20 +2503,20 @@
       <c r="E16" t="s">
         <v>17</v>
       </c>
-      <c r="F16" t="n">
-        <v>15.0</v>
+      <c r="F16">
+        <v>15</v>
       </c>
       <c r="G16" t="s">
         <v>72</v>
       </c>
-      <c r="H16" t="n">
-        <v>0.6513329744338989</v>
-      </c>
-      <c r="I16" t="n">
+      <c r="H16">
+        <v>0.65133297443389893</v>
+      </c>
+      <c r="I16">
         <v>0.30932700634002686</v>
       </c>
-      <c r="J16" t="n">
-        <v>15.0</v>
+      <c r="J16">
+        <v>15</v>
       </c>
       <c r="K16" t="s">
         <v>81</v>
@@ -2194,7 +2528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2210,20 +2544,20 @@
       <c r="E17" t="s">
         <v>17</v>
       </c>
-      <c r="F17" t="n">
-        <v>16.0</v>
+      <c r="F17">
+        <v>16</v>
       </c>
       <c r="G17" t="s">
         <v>84</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17">
         <v>0.43511199951171875</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I17">
         <v>0.47508499026298523</v>
       </c>
-      <c r="J17" t="n">
-        <v>16.0</v>
+      <c r="J17">
+        <v>16</v>
       </c>
       <c r="K17" t="s">
         <v>85</v>
@@ -2235,7 +2569,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2251,20 +2585,20 @@
       <c r="E18" t="s">
         <v>17</v>
       </c>
-      <c r="F18" t="n">
-        <v>19.0</v>
+      <c r="F18">
+        <v>19</v>
       </c>
       <c r="G18" t="s">
         <v>89</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18">
         <v>0.40452900528907776</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18">
         <v>0.20419800281524658</v>
       </c>
-      <c r="J18" t="n">
-        <v>17.0</v>
+      <c r="J18">
+        <v>17</v>
       </c>
       <c r="K18" t="s">
         <v>90</v>
@@ -2276,7 +2610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2292,20 +2626,20 @@
       <c r="E19" t="s">
         <v>17</v>
       </c>
-      <c r="F19" t="n">
-        <v>20.0</v>
+      <c r="F19">
+        <v>20</v>
       </c>
       <c r="G19" t="s">
         <v>94</v>
       </c>
-      <c r="H19" t="n">
-        <v>0.5747089982032776</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.5345240235328674</v>
-      </c>
-      <c r="J19" t="n">
-        <v>18.0</v>
+      <c r="H19">
+        <v>0.57470899820327759</v>
+      </c>
+      <c r="I19">
+        <v>0.53452402353286743</v>
+      </c>
+      <c r="J19">
+        <v>18</v>
       </c>
       <c r="K19" t="s">
         <v>95</v>
@@ -2317,7 +2651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2333,20 +2667,20 @@
       <c r="E20" t="s">
         <v>17</v>
       </c>
-      <c r="F20" t="n">
-        <v>21.0</v>
+      <c r="F20">
+        <v>21</v>
       </c>
       <c r="G20" t="s">
         <v>99</v>
       </c>
-      <c r="H20" t="n">
-        <v>0.5052080154418945</v>
-      </c>
-      <c r="I20" t="n">
+      <c r="H20">
+        <v>0.50520801544189453</v>
+      </c>
+      <c r="I20">
         <v>0.28160199522972107</v>
       </c>
-      <c r="J20" t="n">
-        <v>19.0</v>
+      <c r="J20">
+        <v>19</v>
       </c>
       <c r="K20" t="s">
         <v>100</v>
@@ -2358,7 +2692,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -2374,20 +2708,20 @@
       <c r="E21" t="s">
         <v>17</v>
       </c>
-      <c r="F21" t="n">
-        <v>21.0</v>
+      <c r="F21">
+        <v>21</v>
       </c>
       <c r="G21" t="s">
         <v>99</v>
       </c>
-      <c r="H21" t="n">
-        <v>0.5688329935073853</v>
-      </c>
-      <c r="I21" t="n">
+      <c r="H21">
+        <v>0.56883299350738525</v>
+      </c>
+      <c r="I21">
         <v>0.23854300379753113</v>
       </c>
-      <c r="J21" t="n">
-        <v>20.0</v>
+      <c r="J21">
+        <v>20</v>
       </c>
       <c r="K21" t="s">
         <v>102</v>
@@ -2399,7 +2733,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2415,20 +2749,20 @@
       <c r="E22" t="s">
         <v>17</v>
       </c>
-      <c r="F22" t="n">
-        <v>22.0</v>
+      <c r="F22">
+        <v>22</v>
       </c>
       <c r="G22" t="s">
         <v>106</v>
       </c>
-      <c r="H22" t="n">
-        <v>0.6095319986343384</v>
-      </c>
-      <c r="I22" t="n">
+      <c r="H22">
+        <v>0.60953199863433838</v>
+      </c>
+      <c r="I22">
         <v>0.38180598616600037</v>
       </c>
-      <c r="J22" t="n">
-        <v>21.0</v>
+      <c r="J22">
+        <v>21</v>
       </c>
       <c r="K22" t="s">
         <v>107</v>
@@ -2440,7 +2774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2456,20 +2790,20 @@
       <c r="E23" t="s">
         <v>17</v>
       </c>
-      <c r="F23" t="n">
-        <v>23.0</v>
+      <c r="F23">
+        <v>23</v>
       </c>
       <c r="G23" t="s">
         <v>110</v>
       </c>
-      <c r="H23" t="n">
-        <v>0.4324139952659607</v>
-      </c>
-      <c r="I23" t="n">
+      <c r="H23">
+        <v>0.43241399526596069</v>
+      </c>
+      <c r="I23">
         <v>0.26392701268196106</v>
       </c>
-      <c r="J23" t="n">
-        <v>22.0</v>
+      <c r="J23">
+        <v>22</v>
       </c>
       <c r="K23" t="s">
         <v>111</v>
@@ -2481,7 +2815,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2497,20 +2831,20 @@
       <c r="E24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" t="n">
-        <v>23.0</v>
+      <c r="F24">
+        <v>23</v>
       </c>
       <c r="G24" t="s">
         <v>110</v>
       </c>
-      <c r="H24" t="n">
-        <v>0.3158990144729614</v>
-      </c>
-      <c r="I24" t="n">
+      <c r="H24">
+        <v>0.31589901447296143</v>
+      </c>
+      <c r="I24">
         <v>0.42758598923683167</v>
       </c>
-      <c r="J24" t="n">
-        <v>23.0</v>
+      <c r="J24">
+        <v>23</v>
       </c>
       <c r="K24" t="s">
         <v>114</v>
@@ -2522,7 +2856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2538,20 +2872,20 @@
       <c r="E25" t="s">
         <v>17</v>
       </c>
-      <c r="F25" t="n">
-        <v>23.0</v>
+      <c r="F25">
+        <v>23</v>
       </c>
       <c r="G25" t="s">
         <v>110</v>
       </c>
-      <c r="H25" t="n">
+      <c r="H25">
         <v>0.43733400106430054</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I25">
         <v>0.18402700126171112</v>
       </c>
-      <c r="J25" t="n">
-        <v>24.0</v>
+      <c r="J25">
+        <v>24</v>
       </c>
       <c r="K25" t="s">
         <v>118</v>
@@ -2563,7 +2897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2579,20 +2913,20 @@
       <c r="E26" t="s">
         <v>17</v>
       </c>
-      <c r="F26" t="n">
-        <v>24.0</v>
+      <c r="F26">
+        <v>24</v>
       </c>
       <c r="G26" t="s">
         <v>121</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26">
         <v>0.21154800057411194</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I26">
         <v>0.2476239949464798</v>
       </c>
-      <c r="J26" t="n">
-        <v>25.0</v>
+      <c r="J26">
+        <v>25</v>
       </c>
       <c r="K26" t="s">
         <v>122</v>
@@ -2604,7 +2938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2620,20 +2954,20 @@
       <c r="E27" t="s">
         <v>17</v>
       </c>
-      <c r="F27" t="n">
-        <v>24.0</v>
+      <c r="F27">
+        <v>24</v>
       </c>
       <c r="G27" t="s">
         <v>121</v>
       </c>
-      <c r="H27" t="n">
-        <v>0.4581199884414673</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0.2847230136394501</v>
-      </c>
-      <c r="J27" t="n">
-        <v>26.0</v>
+      <c r="H27">
+        <v>0.45811998844146729</v>
+      </c>
+      <c r="I27">
+        <v>0.28472301363945007</v>
+      </c>
+      <c r="J27">
+        <v>26</v>
       </c>
       <c r="K27" t="s">
         <v>125</v>
@@ -2645,7 +2979,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2661,20 +2995,20 @@
       <c r="E28" t="s">
         <v>17</v>
       </c>
-      <c r="F28" t="n">
-        <v>26.0</v>
+      <c r="F28">
+        <v>26</v>
       </c>
       <c r="G28" t="s">
         <v>128</v>
       </c>
-      <c r="H28" t="n">
-        <v>0.5515710115432739</v>
-      </c>
-      <c r="I28" t="n">
+      <c r="H28">
+        <v>0.55157101154327393</v>
+      </c>
+      <c r="I28">
         <v>0.20184500515460968</v>
       </c>
-      <c r="J28" t="n">
-        <v>27.0</v>
+      <c r="J28">
+        <v>27</v>
       </c>
       <c r="K28" t="s">
         <v>129</v>
@@ -2686,7 +3020,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -2702,20 +3036,20 @@
       <c r="E29" t="s">
         <v>17</v>
       </c>
-      <c r="F29" t="n">
-        <v>26.0</v>
+      <c r="F29">
+        <v>26</v>
       </c>
       <c r="G29" t="s">
         <v>132</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H29">
         <v>0.36283400654792786</v>
       </c>
-      <c r="I29" t="n">
-        <v>0.2996929883956909</v>
-      </c>
-      <c r="J29" t="n">
-        <v>28.0</v>
+      <c r="I29">
+        <v>0.29969298839569092</v>
+      </c>
+      <c r="J29">
+        <v>28</v>
       </c>
       <c r="K29" t="s">
         <v>133</v>
@@ -2727,7 +3061,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2743,20 +3077,20 @@
       <c r="E30" t="s">
         <v>17</v>
       </c>
-      <c r="F30" t="n">
-        <v>27.0</v>
+      <c r="F30">
+        <v>27</v>
       </c>
       <c r="G30" t="s">
         <v>136</v>
       </c>
-      <c r="H30" t="n">
-        <v>0.2389719933271408</v>
-      </c>
-      <c r="I30" t="n">
+      <c r="H30">
+        <v>0.23897199332714081</v>
+      </c>
+      <c r="I30">
         <v>0.20830999314785004</v>
       </c>
-      <c r="J30" t="n">
-        <v>29.0</v>
+      <c r="J30">
+        <v>29</v>
       </c>
       <c r="K30" t="s">
         <v>137</v>
@@ -2768,7 +3102,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2784,20 +3118,20 @@
       <c r="E31" t="s">
         <v>17</v>
       </c>
-      <c r="F31" t="n">
-        <v>27.0</v>
+      <c r="F31">
+        <v>27</v>
       </c>
       <c r="G31" t="s">
         <v>136</v>
       </c>
-      <c r="H31" t="n">
+      <c r="H31">
         <v>0.27779099345207214</v>
       </c>
-      <c r="I31" t="n">
-        <v>0.2930009961128235</v>
-      </c>
-      <c r="J31" t="n">
-        <v>30.0</v>
+      <c r="I31">
+        <v>0.29300099611282349</v>
+      </c>
+      <c r="J31">
+        <v>30</v>
       </c>
       <c r="K31" t="s">
         <v>141</v>
@@ -2809,7 +3143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -2825,20 +3159,20 @@
       <c r="E32" t="s">
         <v>17</v>
       </c>
-      <c r="F32" t="n">
-        <v>28.0</v>
+      <c r="F32">
+        <v>28</v>
       </c>
       <c r="G32" t="s">
         <v>144</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H32">
         <v>0.5805240273475647</v>
       </c>
-      <c r="I32" t="n">
-        <v>0.2410220056772232</v>
-      </c>
-      <c r="J32" t="n">
-        <v>31.0</v>
+      <c r="I32">
+        <v>0.24102200567722321</v>
+      </c>
+      <c r="J32">
+        <v>31</v>
       </c>
       <c r="K32" t="s">
         <v>145</v>
@@ -2850,7 +3184,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -2866,20 +3200,20 @@
       <c r="E33" t="s">
         <v>17</v>
       </c>
-      <c r="F33" t="n">
-        <v>28.0</v>
+      <c r="F33">
+        <v>28</v>
       </c>
       <c r="G33" t="s">
         <v>148</v>
       </c>
-      <c r="H33" t="n">
-        <v>0.6651250123977661</v>
-      </c>
-      <c r="I33" t="n">
+      <c r="H33">
+        <v>0.66512501239776611</v>
+      </c>
+      <c r="I33">
         <v>0.19724899530410767</v>
       </c>
-      <c r="J33" t="n">
-        <v>32.0</v>
+      <c r="J33">
+        <v>32</v>
       </c>
       <c r="K33" t="s">
         <v>149</v>
@@ -2891,7 +3225,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -2907,20 +3241,20 @@
       <c r="E34" t="s">
         <v>17</v>
       </c>
-      <c r="F34" t="n">
-        <v>29.0</v>
+      <c r="F34">
+        <v>29</v>
       </c>
       <c r="G34" t="s">
         <v>152</v>
       </c>
-      <c r="H34" t="n">
-        <v>0.61319899559021</v>
-      </c>
-      <c r="I34" t="n">
+      <c r="H34">
+        <v>0.61319899559020996</v>
+      </c>
+      <c r="I34">
         <v>0.14354999363422394</v>
       </c>
-      <c r="J34" t="n">
-        <v>33.0</v>
+      <c r="J34">
+        <v>33</v>
       </c>
       <c r="K34" t="s">
         <v>153</v>
@@ -2932,7 +3266,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -2948,20 +3282,20 @@
       <c r="E35" t="s">
         <v>17</v>
       </c>
-      <c r="F35" t="n">
-        <v>29.0</v>
+      <c r="F35">
+        <v>29</v>
       </c>
       <c r="G35" t="s">
         <v>152</v>
       </c>
-      <c r="H35" t="n">
+      <c r="H35">
         <v>0.6098560094833374</v>
       </c>
-      <c r="I35" t="n">
+      <c r="I35">
         <v>0.2113330066204071</v>
       </c>
-      <c r="J35" t="n">
-        <v>34.0</v>
+      <c r="J35">
+        <v>34</v>
       </c>
       <c r="K35" t="s">
         <v>156</v>
@@ -2973,7 +3307,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -2989,20 +3323,20 @@
       <c r="E36" t="s">
         <v>17</v>
       </c>
-      <c r="F36" t="n">
-        <v>29.0</v>
+      <c r="F36">
+        <v>29</v>
       </c>
       <c r="G36" t="s">
         <v>152</v>
       </c>
-      <c r="H36" t="n">
+      <c r="H36">
         <v>0.19258899986743927</v>
       </c>
-      <c r="I36" t="n">
-        <v>0.3297399878501892</v>
-      </c>
-      <c r="J36" t="n">
-        <v>35.0</v>
+      <c r="I36">
+        <v>0.32973998785018921</v>
+      </c>
+      <c r="J36">
+        <v>35</v>
       </c>
       <c r="K36" t="s">
         <v>160</v>
@@ -3014,7 +3348,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -3030,20 +3364,20 @@
       <c r="E37" t="s">
         <v>17</v>
       </c>
-      <c r="F37" t="n">
-        <v>30.0</v>
+      <c r="F37">
+        <v>30</v>
       </c>
       <c r="G37" t="s">
         <v>163</v>
       </c>
-      <c r="H37" t="n">
-        <v>0.5589730143547058</v>
-      </c>
-      <c r="I37" t="n">
+      <c r="H37">
+        <v>0.55897301435470581</v>
+      </c>
+      <c r="I37">
         <v>0.1998240053653717</v>
       </c>
-      <c r="J37" t="n">
-        <v>36.0</v>
+      <c r="J37">
+        <v>36</v>
       </c>
       <c r="K37" t="s">
         <v>164</v>
@@ -3055,7 +3389,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -3071,20 +3405,20 @@
       <c r="E38" t="s">
         <v>17</v>
       </c>
-      <c r="F38" t="n">
-        <v>30.0</v>
+      <c r="F38">
+        <v>30</v>
       </c>
       <c r="G38" t="s">
         <v>168</v>
       </c>
-      <c r="H38" t="n">
-        <v>0.3752390146255493</v>
-      </c>
-      <c r="I38" t="n">
+      <c r="H38">
+        <v>0.37523901462554932</v>
+      </c>
+      <c r="I38">
         <v>0.1708189994096756</v>
       </c>
-      <c r="J38" t="n">
-        <v>37.0</v>
+      <c r="J38">
+        <v>37</v>
       </c>
       <c r="K38" t="s">
         <v>169</v>
@@ -3096,7 +3430,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -3112,20 +3446,20 @@
       <c r="E39" t="s">
         <v>17</v>
       </c>
-      <c r="F39" t="n">
-        <v>31.0</v>
+      <c r="F39">
+        <v>31</v>
       </c>
       <c r="G39" t="s">
         <v>172</v>
       </c>
-      <c r="H39" t="n">
+      <c r="H39">
         <v>0.4040600061416626</v>
       </c>
-      <c r="I39" t="n">
+      <c r="I39">
         <v>0.221343994140625</v>
       </c>
-      <c r="J39" t="n">
-        <v>38.0</v>
+      <c r="J39">
+        <v>38</v>
       </c>
       <c r="K39" t="s">
         <v>173</v>
@@ -3137,7 +3471,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -3153,20 +3487,20 @@
       <c r="E40" t="s">
         <v>17</v>
       </c>
-      <c r="F40" t="n">
-        <v>31.0</v>
+      <c r="F40">
+        <v>31</v>
       </c>
       <c r="G40" t="s">
         <v>176</v>
       </c>
-      <c r="H40" t="n">
-        <v>0.4284310042858124</v>
-      </c>
-      <c r="I40" t="n">
+      <c r="H40">
+        <v>0.42843100428581238</v>
+      </c>
+      <c r="I40">
         <v>0.28393200039863586</v>
       </c>
-      <c r="J40" t="n">
-        <v>39.0</v>
+      <c r="J40">
+        <v>39</v>
       </c>
       <c r="K40" t="s">
         <v>177</v>
@@ -3178,7 +3512,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -3194,20 +3528,20 @@
       <c r="E41" t="s">
         <v>17</v>
       </c>
-      <c r="F41" t="n">
-        <v>32.0</v>
+      <c r="F41">
+        <v>32</v>
       </c>
       <c r="G41" t="s">
         <v>180</v>
       </c>
-      <c r="H41" t="n">
-        <v>0.5190950036048889</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0.2533409893512726</v>
-      </c>
-      <c r="J41" t="n">
-        <v>40.0</v>
+      <c r="H41">
+        <v>0.51909500360488892</v>
+      </c>
+      <c r="I41">
+        <v>0.25334098935127258</v>
+      </c>
+      <c r="J41">
+        <v>40</v>
       </c>
       <c r="K41" t="s">
         <v>181</v>
@@ -3219,7 +3553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -3235,20 +3569,20 @@
       <c r="E42" t="s">
         <v>17</v>
       </c>
-      <c r="F42" t="n">
-        <v>32.0</v>
+      <c r="F42">
+        <v>32</v>
       </c>
       <c r="G42" t="s">
         <v>185</v>
       </c>
-      <c r="H42" t="n">
-        <v>0.5477510094642639</v>
-      </c>
-      <c r="I42" t="n">
+      <c r="H42">
+        <v>0.54775100946426392</v>
+      </c>
+      <c r="I42">
         <v>0.2268809974193573</v>
       </c>
-      <c r="J42" t="n">
-        <v>41.0</v>
+      <c r="J42">
+        <v>41</v>
       </c>
       <c r="K42" t="s">
         <v>186</v>
@@ -3260,7 +3594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -3276,20 +3610,20 @@
       <c r="E43" t="s">
         <v>17</v>
       </c>
-      <c r="F43" t="n">
-        <v>33.0</v>
+      <c r="F43">
+        <v>33</v>
       </c>
       <c r="G43" t="s">
         <v>189</v>
       </c>
-      <c r="H43" t="n">
-        <v>0.4424870014190674</v>
-      </c>
-      <c r="I43" t="n">
+      <c r="H43">
+        <v>0.44248700141906738</v>
+      </c>
+      <c r="I43">
         <v>0.23048000037670135</v>
       </c>
-      <c r="J43" t="n">
-        <v>42.0</v>
+      <c r="J43">
+        <v>42</v>
       </c>
       <c r="K43" t="s">
         <v>190</v>
@@ -3301,7 +3635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -3317,20 +3651,20 @@
       <c r="E44" t="s">
         <v>17</v>
       </c>
-      <c r="F44" t="n">
-        <v>33.0</v>
+      <c r="F44">
+        <v>33</v>
       </c>
       <c r="G44" t="s">
         <v>194</v>
       </c>
-      <c r="H44" t="n">
-        <v>0.5500180125236511</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0.2732119858264923</v>
-      </c>
-      <c r="J44" t="n">
-        <v>43.0</v>
+      <c r="H44">
+        <v>0.55001801252365112</v>
+      </c>
+      <c r="I44">
+        <v>0.27321198582649231</v>
+      </c>
+      <c r="J44">
+        <v>43</v>
       </c>
       <c r="K44" t="s">
         <v>195</v>
@@ -3342,7 +3676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -3358,20 +3692,20 @@
       <c r="E45" t="s">
         <v>17</v>
       </c>
-      <c r="F45" t="n">
-        <v>33.0</v>
+      <c r="F45">
+        <v>33</v>
       </c>
       <c r="G45" t="s">
         <v>194</v>
       </c>
-      <c r="H45" t="n">
+      <c r="H45">
         <v>0.4467490017414093</v>
       </c>
-      <c r="I45" t="n">
+      <c r="I45">
         <v>0.24743899703025818</v>
       </c>
-      <c r="J45" t="n">
-        <v>44.0</v>
+      <c r="J45">
+        <v>44</v>
       </c>
       <c r="K45" t="s">
         <v>198</v>
@@ -3383,7 +3717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -3399,20 +3733,20 @@
       <c r="E46" t="s">
         <v>17</v>
       </c>
-      <c r="F46" t="n">
-        <v>33.0</v>
+      <c r="F46">
+        <v>33</v>
       </c>
       <c r="G46" t="s">
         <v>194</v>
       </c>
-      <c r="H46" t="n">
-        <v>0.3787370026111603</v>
-      </c>
-      <c r="I46" t="n">
+      <c r="H46">
+        <v>0.37873700261116028</v>
+      </c>
+      <c r="I46">
         <v>0.21008500456809998</v>
       </c>
-      <c r="J46" t="n">
-        <v>45.0</v>
+      <c r="J46">
+        <v>45</v>
       </c>
       <c r="K46" t="s">
         <v>202</v>
@@ -3424,7 +3758,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -3440,20 +3774,20 @@
       <c r="E47" t="s">
         <v>17</v>
       </c>
-      <c r="F47" t="n">
-        <v>34.0</v>
+      <c r="F47">
+        <v>34</v>
       </c>
       <c r="G47" t="s">
         <v>206</v>
       </c>
-      <c r="H47" t="n">
+      <c r="H47">
         <v>0.4942300021648407</v>
       </c>
-      <c r="I47" t="n">
+      <c r="I47">
         <v>0.14772599935531616</v>
       </c>
-      <c r="J47" t="n">
-        <v>46.0</v>
+      <c r="J47">
+        <v>46</v>
       </c>
       <c r="K47" t="s">
         <v>207</v>
@@ -3465,7 +3799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -3481,20 +3815,20 @@
       <c r="E48" t="s">
         <v>17</v>
       </c>
-      <c r="F48" t="n">
-        <v>34.0</v>
+      <c r="F48">
+        <v>34</v>
       </c>
       <c r="G48" t="s">
         <v>211</v>
       </c>
-      <c r="H48" t="n">
+      <c r="H48">
         <v>0.22058700025081635</v>
       </c>
-      <c r="I48" t="n">
+      <c r="I48">
         <v>0.21617799997329712</v>
       </c>
-      <c r="J48" t="n">
-        <v>47.0</v>
+      <c r="J48">
+        <v>47</v>
       </c>
       <c r="K48" t="s">
         <v>212</v>
@@ -3506,7 +3840,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -3522,20 +3856,20 @@
       <c r="E49" t="s">
         <v>17</v>
       </c>
-      <c r="F49" t="n">
-        <v>35.0</v>
+      <c r="F49">
+        <v>35</v>
       </c>
       <c r="G49" t="s">
         <v>215</v>
       </c>
-      <c r="H49" t="n">
-        <v>0.4367940127849579</v>
-      </c>
-      <c r="I49" t="n">
+      <c r="H49">
+        <v>0.43679401278495789</v>
+      </c>
+      <c r="I49">
         <v>0.19729499518871307</v>
       </c>
-      <c r="J49" t="n">
-        <v>48.0</v>
+      <c r="J49">
+        <v>48</v>
       </c>
       <c r="K49" t="s">
         <v>216</v>
@@ -3547,7 +3881,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -3563,20 +3897,20 @@
       <c r="E50" t="s">
         <v>17</v>
       </c>
-      <c r="F50" t="n">
-        <v>35.0</v>
+      <c r="F50">
+        <v>35</v>
       </c>
       <c r="G50" t="s">
         <v>215</v>
       </c>
-      <c r="H50" t="n">
-        <v>0.5721650123596191</v>
-      </c>
-      <c r="I50" t="n">
+      <c r="H50">
+        <v>0.57216501235961914</v>
+      </c>
+      <c r="I50">
         <v>0.18042400479316711</v>
       </c>
-      <c r="J50" t="n">
-        <v>49.0</v>
+      <c r="J50">
+        <v>49</v>
       </c>
       <c r="K50" t="s">
         <v>220</v>
@@ -3588,7 +3922,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -3604,20 +3938,20 @@
       <c r="E51" t="s">
         <v>17</v>
       </c>
-      <c r="F51" t="n">
-        <v>35.0</v>
+      <c r="F51">
+        <v>35</v>
       </c>
       <c r="G51" t="s">
         <v>223</v>
       </c>
-      <c r="H51" t="n">
-        <v>0.550400972366333</v>
-      </c>
-      <c r="I51" t="n">
+      <c r="H51">
+        <v>0.55040097236633301</v>
+      </c>
+      <c r="I51">
         <v>0.15516500174999237</v>
       </c>
-      <c r="J51" t="n">
-        <v>50.0</v>
+      <c r="J51">
+        <v>50</v>
       </c>
       <c r="K51" t="s">
         <v>224</v>
@@ -3629,7 +3963,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -3645,20 +3979,20 @@
       <c r="E52" t="s">
         <v>17</v>
       </c>
-      <c r="F52" t="n">
-        <v>36.0</v>
+      <c r="F52">
+        <v>36</v>
       </c>
       <c r="G52" t="s">
         <v>227</v>
       </c>
-      <c r="H52" t="n">
+      <c r="H52">
         <v>0.47011199593544006</v>
       </c>
-      <c r="I52" t="n">
+      <c r="I52">
         <v>0.20512500405311584</v>
       </c>
-      <c r="J52" t="n">
-        <v>51.0</v>
+      <c r="J52">
+        <v>51</v>
       </c>
       <c r="K52" t="s">
         <v>228</v>
@@ -3670,7 +4004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -3686,20 +4020,20 @@
       <c r="E53" t="s">
         <v>17</v>
       </c>
-      <c r="F53" t="n">
-        <v>37.0</v>
+      <c r="F53">
+        <v>37</v>
       </c>
       <c r="G53" t="s">
         <v>231</v>
       </c>
-      <c r="H53" t="n">
+      <c r="H53">
         <v>0.43899399042129517</v>
       </c>
-      <c r="I53" t="n">
+      <c r="I53">
         <v>0.2012770026922226</v>
       </c>
-      <c r="J53" t="n">
-        <v>52.0</v>
+      <c r="J53">
+        <v>52</v>
       </c>
       <c r="K53" t="s">
         <v>232</v>
@@ -3711,7 +4045,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -3727,20 +4061,20 @@
       <c r="E54" t="s">
         <v>17</v>
       </c>
-      <c r="F54" t="n">
-        <v>38.0</v>
+      <c r="F54">
+        <v>38</v>
       </c>
       <c r="G54" t="s">
         <v>235</v>
       </c>
-      <c r="H54" t="n">
-        <v>0.6205009818077087</v>
-      </c>
-      <c r="I54" t="n">
+      <c r="H54">
+        <v>0.62050098180770874</v>
+      </c>
+      <c r="I54">
         <v>0.18775899708271027</v>
       </c>
-      <c r="J54" t="n">
-        <v>53.0</v>
+      <c r="J54">
+        <v>53</v>
       </c>
       <c r="K54" t="s">
         <v>236</v>
@@ -3752,7 +4086,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -3768,20 +4102,20 @@
       <c r="E55" t="s">
         <v>17</v>
       </c>
-      <c r="F55" t="n">
-        <v>38.0</v>
+      <c r="F55">
+        <v>38</v>
       </c>
       <c r="G55" t="s">
         <v>235</v>
       </c>
-      <c r="H55" t="n">
-        <v>0.3630940020084381</v>
-      </c>
-      <c r="I55" t="n">
+      <c r="H55">
+        <v>0.36309400200843811</v>
+      </c>
+      <c r="I55">
         <v>0.24005399644374847</v>
       </c>
-      <c r="J55" t="n">
-        <v>54.0</v>
+      <c r="J55">
+        <v>54</v>
       </c>
       <c r="K55" t="s">
         <v>239</v>
@@ -3793,7 +4127,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -3809,20 +4143,20 @@
       <c r="E56" t="s">
         <v>17</v>
       </c>
-      <c r="F56" t="n">
-        <v>39.0</v>
+      <c r="F56">
+        <v>39</v>
       </c>
       <c r="G56" t="s">
         <v>242</v>
       </c>
-      <c r="H56" t="n">
-        <v>0.5874630212783813</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0.1659500002861023</v>
-      </c>
-      <c r="J56" t="n">
-        <v>55.0</v>
+      <c r="H56">
+        <v>0.58746302127838135</v>
+      </c>
+      <c r="I56">
+        <v>0.16595000028610229</v>
+      </c>
+      <c r="J56">
+        <v>55</v>
       </c>
       <c r="K56" t="s">
         <v>243</v>
@@ -3834,7 +4168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -3850,20 +4184,20 @@
       <c r="E57" t="s">
         <v>17</v>
       </c>
-      <c r="F57" t="n">
-        <v>39.0</v>
+      <c r="F57">
+        <v>39</v>
       </c>
       <c r="G57" t="s">
         <v>242</v>
       </c>
-      <c r="H57" t="n">
-        <v>0.6750739812850952</v>
-      </c>
-      <c r="I57" t="n">
+      <c r="H57">
+        <v>0.67507398128509521</v>
+      </c>
+      <c r="I57">
         <v>0.17146900296211243</v>
       </c>
-      <c r="J57" t="n">
-        <v>56.0</v>
+      <c r="J57">
+        <v>56</v>
       </c>
       <c r="K57" t="s">
         <v>247</v>
@@ -3875,7 +4209,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -3891,20 +4225,20 @@
       <c r="E58" t="s">
         <v>17</v>
       </c>
-      <c r="F58" t="n">
-        <v>39.0</v>
+      <c r="F58">
+        <v>39</v>
       </c>
       <c r="G58" t="s">
         <v>250</v>
       </c>
-      <c r="H58" t="n">
+      <c r="H58">
         <v>0.18226100504398346</v>
       </c>
-      <c r="I58" t="n">
+      <c r="I58">
         <v>0.16366399824619293</v>
       </c>
-      <c r="J58" t="n">
-        <v>57.0</v>
+      <c r="J58">
+        <v>57</v>
       </c>
       <c r="K58" t="s">
         <v>251</v>
@@ -3916,7 +4250,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -3932,20 +4266,20 @@
       <c r="E59" t="s">
         <v>17</v>
       </c>
-      <c r="F59" t="n">
-        <v>39.0</v>
+      <c r="F59">
+        <v>39</v>
       </c>
       <c r="G59" t="s">
         <v>254</v>
       </c>
-      <c r="H59" t="n">
-        <v>0.3685249984264374</v>
-      </c>
-      <c r="I59" t="n">
+      <c r="H59">
+        <v>0.36852499842643738</v>
+      </c>
+      <c r="I59">
         <v>0.24173499643802643</v>
       </c>
-      <c r="J59" t="n">
-        <v>58.0</v>
+      <c r="J59">
+        <v>58</v>
       </c>
       <c r="K59" t="s">
         <v>255</v>
@@ -3957,7 +4291,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -3973,20 +4307,20 @@
       <c r="E60" t="s">
         <v>17</v>
       </c>
-      <c r="F60" t="n">
-        <v>40.0</v>
+      <c r="F60">
+        <v>40</v>
       </c>
       <c r="G60" t="s">
         <v>258</v>
       </c>
-      <c r="H60" t="n">
+      <c r="H60">
         <v>0.34213700890541077</v>
       </c>
-      <c r="I60" t="n">
+      <c r="I60">
         <v>0.13651199638843536</v>
       </c>
-      <c r="J60" t="n">
-        <v>59.0</v>
+      <c r="J60">
+        <v>59</v>
       </c>
       <c r="K60" t="s">
         <v>259</v>
@@ -3998,7 +4332,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -4014,20 +4348,20 @@
       <c r="E61" t="s">
         <v>17</v>
       </c>
-      <c r="F61" t="n">
-        <v>40.0</v>
+      <c r="F61">
+        <v>40</v>
       </c>
       <c r="G61" t="s">
         <v>263</v>
       </c>
-      <c r="H61" t="n">
-        <v>0.5215129852294922</v>
-      </c>
-      <c r="I61" t="n">
+      <c r="H61">
+        <v>0.52151298522949219</v>
+      </c>
+      <c r="I61">
         <v>0.15008099377155304</v>
       </c>
-      <c r="J61" t="n">
-        <v>60.0</v>
+      <c r="J61">
+        <v>60</v>
       </c>
       <c r="K61" t="s">
         <v>264</v>
@@ -4039,7 +4373,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -4055,20 +4389,20 @@
       <c r="E62" t="s">
         <v>17</v>
       </c>
-      <c r="F62" t="n">
-        <v>40.0</v>
+      <c r="F62">
+        <v>40</v>
       </c>
       <c r="G62" t="s">
         <v>258</v>
       </c>
-      <c r="H62" t="n">
-        <v>0.2310830056667328</v>
-      </c>
-      <c r="I62" t="n">
+      <c r="H62">
+        <v>0.23108300566673279</v>
+      </c>
+      <c r="I62">
         <v>0.16609600186347961</v>
       </c>
-      <c r="J62" t="n">
-        <v>61.0</v>
+      <c r="J62">
+        <v>61</v>
       </c>
       <c r="K62" t="s">
         <v>267</v>
@@ -4080,7 +4414,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -4096,20 +4430,20 @@
       <c r="E63" t="s">
         <v>17</v>
       </c>
-      <c r="F63" t="n">
-        <v>41.0</v>
+      <c r="F63">
+        <v>41</v>
       </c>
       <c r="G63" t="s">
         <v>270</v>
       </c>
-      <c r="H63" t="n">
+      <c r="H63">
         <v>0.3771359920501709</v>
       </c>
-      <c r="I63" t="n">
+      <c r="I63">
         <v>0.12748700380325317</v>
       </c>
-      <c r="J63" t="n">
-        <v>62.0</v>
+      <c r="J63">
+        <v>62</v>
       </c>
       <c r="K63" t="s">
         <v>271</v>
@@ -4121,7 +4455,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -4137,20 +4471,20 @@
       <c r="E64" t="s">
         <v>17</v>
       </c>
-      <c r="F64" t="n">
-        <v>41.0</v>
+      <c r="F64">
+        <v>41</v>
       </c>
       <c r="G64" t="s">
         <v>270</v>
       </c>
-      <c r="H64" t="n">
-        <v>0.5572050213813782</v>
-      </c>
-      <c r="I64" t="n">
+      <c r="H64">
+        <v>0.55720502138137817</v>
+      </c>
+      <c r="I64">
         <v>0.17568999528884888</v>
       </c>
-      <c r="J64" t="n">
-        <v>63.0</v>
+      <c r="J64">
+        <v>63</v>
       </c>
       <c r="K64" t="s">
         <v>274</v>
@@ -4162,7 +4496,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -4178,20 +4512,20 @@
       <c r="E65" t="s">
         <v>17</v>
       </c>
-      <c r="F65" t="n">
-        <v>42.0</v>
+      <c r="F65">
+        <v>42</v>
       </c>
       <c r="G65" t="s">
         <v>277</v>
       </c>
-      <c r="H65" t="n">
-        <v>0.6209229826927185</v>
-      </c>
-      <c r="I65" t="n">
-        <v>0.1444990038871765</v>
-      </c>
-      <c r="J65" t="n">
-        <v>64.0</v>
+      <c r="H65">
+        <v>0.62092298269271851</v>
+      </c>
+      <c r="I65">
+        <v>0.14449900388717651</v>
+      </c>
+      <c r="J65">
+        <v>64</v>
       </c>
       <c r="K65" t="s">
         <v>278</v>
@@ -4203,7 +4537,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -4219,20 +4553,20 @@
       <c r="E66" t="s">
         <v>17</v>
       </c>
-      <c r="F66" t="n">
-        <v>42.0</v>
+      <c r="F66">
+        <v>42</v>
       </c>
       <c r="G66" t="s">
         <v>282</v>
       </c>
-      <c r="H66" t="n">
+      <c r="H66">
         <v>0.40560799837112427</v>
       </c>
-      <c r="I66" t="n">
+      <c r="I66">
         <v>0.23708400130271912</v>
       </c>
-      <c r="J66" t="n">
-        <v>65.0</v>
+      <c r="J66">
+        <v>65</v>
       </c>
       <c r="K66" t="s">
         <v>271</v>
@@ -4244,7 +4578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -4260,20 +4594,20 @@
       <c r="E67" t="s">
         <v>17</v>
       </c>
-      <c r="F67" t="n">
-        <v>42.0</v>
+      <c r="F67">
+        <v>42</v>
       </c>
       <c r="G67" t="s">
         <v>282</v>
       </c>
-      <c r="H67" t="n">
-        <v>0.5734959840774536</v>
-      </c>
-      <c r="I67" t="n">
+      <c r="H67">
+        <v>0.57349598407745361</v>
+      </c>
+      <c r="I67">
         <v>0.14475299417972565</v>
       </c>
-      <c r="J67" t="n">
-        <v>66.0</v>
+      <c r="J67">
+        <v>66</v>
       </c>
       <c r="K67" t="s">
         <v>285</v>
@@ -4285,7 +4619,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -4301,20 +4635,20 @@
       <c r="E68" t="s">
         <v>17</v>
       </c>
-      <c r="F68" t="n">
-        <v>44.0</v>
+      <c r="F68">
+        <v>44</v>
       </c>
       <c r="G68" t="s">
         <v>289</v>
       </c>
-      <c r="H68" t="n">
-        <v>0.5325999855995178</v>
-      </c>
-      <c r="I68" t="n">
+      <c r="H68">
+        <v>0.53259998559951782</v>
+      </c>
+      <c r="I68">
         <v>0.20031200349330902</v>
       </c>
-      <c r="J68" t="n">
-        <v>67.0</v>
+      <c r="J68">
+        <v>67</v>
       </c>
       <c r="K68" t="s">
         <v>290</v>
@@ -4326,7 +4660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -4342,20 +4676,20 @@
       <c r="E69" t="s">
         <v>17</v>
       </c>
-      <c r="F69" t="n">
-        <v>44.0</v>
+      <c r="F69">
+        <v>44</v>
       </c>
       <c r="G69" t="s">
         <v>289</v>
       </c>
-      <c r="H69" t="n">
-        <v>0.6567869782447815</v>
-      </c>
-      <c r="I69" t="n">
+      <c r="H69">
+        <v>0.65678697824478149</v>
+      </c>
+      <c r="I69">
         <v>0.16937699913978577</v>
       </c>
-      <c r="J69" t="n">
-        <v>68.0</v>
+      <c r="J69">
+        <v>68</v>
       </c>
       <c r="K69" t="s">
         <v>137</v>
@@ -4367,7 +4701,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -4383,20 +4717,20 @@
       <c r="E70" t="s">
         <v>17</v>
       </c>
-      <c r="F70" t="n">
-        <v>44.0</v>
+      <c r="F70">
+        <v>44</v>
       </c>
       <c r="G70" t="s">
         <v>289</v>
       </c>
-      <c r="H70" t="n">
-        <v>0.4815619885921478</v>
-      </c>
-      <c r="I70" t="n">
+      <c r="H70">
+        <v>0.48156198859214783</v>
+      </c>
+      <c r="I70">
         <v>0.20215700566768646</v>
       </c>
-      <c r="J70" t="n">
-        <v>69.0</v>
+      <c r="J70">
+        <v>69</v>
       </c>
       <c r="K70" t="s">
         <v>297</v>
@@ -4408,7 +4742,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -4424,20 +4758,20 @@
       <c r="E71" t="s">
         <v>17</v>
       </c>
-      <c r="F71" t="n">
-        <v>45.0</v>
+      <c r="F71">
+        <v>45</v>
       </c>
       <c r="G71" t="s">
         <v>301</v>
       </c>
-      <c r="H71" t="n">
-        <v>0.3132700026035309</v>
-      </c>
-      <c r="I71" t="n">
+      <c r="H71">
+        <v>0.31327000260353088</v>
+      </c>
+      <c r="I71">
         <v>0.15031099319458008</v>
       </c>
-      <c r="J71" t="n">
-        <v>70.0</v>
+      <c r="J71">
+        <v>70</v>
       </c>
       <c r="K71" t="s">
         <v>302</v>
@@ -4449,7 +4783,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -4465,20 +4799,20 @@
       <c r="E72" t="s">
         <v>17</v>
       </c>
-      <c r="F72" t="n">
-        <v>47.0</v>
+      <c r="F72">
+        <v>47</v>
       </c>
       <c r="G72" t="s">
         <v>305</v>
       </c>
-      <c r="H72" t="n">
+      <c r="H72">
         <v>0.48000800609588623</v>
       </c>
-      <c r="I72" t="n">
+      <c r="I72">
         <v>0.19152699410915375</v>
       </c>
-      <c r="J72" t="n">
-        <v>71.0</v>
+      <c r="J72">
+        <v>71</v>
       </c>
       <c r="K72" t="s">
         <v>306</v>
@@ -4490,7 +4824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>13</v>
       </c>
@@ -4506,20 +4840,20 @@
       <c r="E73" t="s">
         <v>17</v>
       </c>
-      <c r="F73" t="n">
-        <v>47.0</v>
+      <c r="F73">
+        <v>47</v>
       </c>
       <c r="G73" t="s">
         <v>309</v>
       </c>
-      <c r="H73" t="n">
-        <v>0.5990380048751831</v>
-      </c>
-      <c r="I73" t="n">
-        <v>0.09884549677371979</v>
-      </c>
-      <c r="J73" t="n">
-        <v>72.0</v>
+      <c r="H73">
+        <v>0.59903800487518311</v>
+      </c>
+      <c r="I73">
+        <v>9.8845496773719788E-2</v>
+      </c>
+      <c r="J73">
+        <v>72</v>
       </c>
       <c r="K73" t="s">
         <v>310</v>
@@ -4531,7 +4865,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -4547,20 +4881,20 @@
       <c r="E74" t="s">
         <v>17</v>
       </c>
-      <c r="F74" t="n">
-        <v>47.0</v>
+      <c r="F74">
+        <v>47</v>
       </c>
       <c r="G74" t="s">
         <v>309</v>
       </c>
-      <c r="H74" t="n">
-        <v>0.6128529906272888</v>
-      </c>
-      <c r="I74" t="n">
+      <c r="H74">
+        <v>0.61285299062728882</v>
+      </c>
+      <c r="I74">
         <v>0.11427299678325653</v>
       </c>
-      <c r="J74" t="n">
-        <v>73.0</v>
+      <c r="J74">
+        <v>73</v>
       </c>
       <c r="K74" t="s">
         <v>314</v>
@@ -4572,7 +4906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -4588,20 +4922,20 @@
       <c r="E75" t="s">
         <v>17</v>
       </c>
-      <c r="F75" t="n">
-        <v>48.0</v>
+      <c r="F75">
+        <v>48</v>
       </c>
       <c r="G75" t="s">
         <v>317</v>
       </c>
-      <c r="H75" t="n">
-        <v>0.3371039927005768</v>
-      </c>
-      <c r="I75" t="n">
+      <c r="H75">
+        <v>0.33710399270057678</v>
+      </c>
+      <c r="I75">
         <v>0.18239599466323853</v>
       </c>
-      <c r="J75" t="n">
-        <v>74.0</v>
+      <c r="J75">
+        <v>74</v>
       </c>
       <c r="K75" t="s">
         <v>318</v>
@@ -4613,7 +4947,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -4629,20 +4963,20 @@
       <c r="E76" t="s">
         <v>17</v>
       </c>
-      <c r="F76" t="n">
-        <v>50.0</v>
+      <c r="F76">
+        <v>50</v>
       </c>
       <c r="G76" t="s">
         <v>321</v>
       </c>
-      <c r="H76" t="n">
-        <v>0.5377489924430847</v>
-      </c>
-      <c r="I76" t="n">
+      <c r="H76">
+        <v>0.53774899244308472</v>
+      </c>
+      <c r="I76">
         <v>0.22548800706863403</v>
       </c>
-      <c r="J76" t="n">
-        <v>75.0</v>
+      <c r="J76">
+        <v>75</v>
       </c>
       <c r="K76" t="s">
         <v>322</v>
@@ -4654,7 +4988,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -4670,20 +5004,20 @@
       <c r="E77" t="s">
         <v>17</v>
       </c>
-      <c r="F77" t="n">
-        <v>50.0</v>
+      <c r="F77">
+        <v>50</v>
       </c>
       <c r="G77" t="s">
         <v>326</v>
       </c>
-      <c r="H77" t="n">
-        <v>0.57157301902771</v>
-      </c>
-      <c r="I77" t="n">
+      <c r="H77">
+        <v>0.57157301902770996</v>
+      </c>
+      <c r="I77">
         <v>0.13028199970722198</v>
       </c>
-      <c r="J77" t="n">
-        <v>76.0</v>
+      <c r="J77">
+        <v>76</v>
       </c>
       <c r="K77" t="s">
         <v>327</v>
@@ -4695,7 +5029,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -4711,20 +5045,20 @@
       <c r="E78" t="s">
         <v>17</v>
       </c>
-      <c r="F78" t="n">
-        <v>50.0</v>
+      <c r="F78">
+        <v>50</v>
       </c>
       <c r="G78" t="s">
         <v>329</v>
       </c>
-      <c r="H78" t="n">
+      <c r="H78">
         <v>0.43317100405693054</v>
       </c>
-      <c r="I78" t="n">
+      <c r="I78">
         <v>0.13728199899196625</v>
       </c>
-      <c r="J78" t="n">
-        <v>77.0</v>
+      <c r="J78">
+        <v>77</v>
       </c>
       <c r="K78" t="s">
         <v>330</v>
@@ -4736,7 +5070,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>13</v>
       </c>
@@ -4752,20 +5086,20 @@
       <c r="E79" t="s">
         <v>17</v>
       </c>
-      <c r="F79" t="n">
-        <v>51.0</v>
+      <c r="F79">
+        <v>51</v>
       </c>
       <c r="G79" t="s">
         <v>334</v>
       </c>
-      <c r="H79" t="n">
-        <v>0.477400004863739</v>
-      </c>
-      <c r="I79" t="n">
+      <c r="H79">
+        <v>0.47740000486373901</v>
+      </c>
+      <c r="I79">
         <v>0.17314499616622925</v>
       </c>
-      <c r="J79" t="n">
-        <v>78.0</v>
+      <c r="J79">
+        <v>78</v>
       </c>
       <c r="K79" t="s">
         <v>335</v>
@@ -4777,7 +5111,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>13</v>
       </c>
@@ -4793,20 +5127,20 @@
       <c r="E80" t="s">
         <v>17</v>
       </c>
-      <c r="F80" t="n">
-        <v>51.0</v>
+      <c r="F80">
+        <v>51</v>
       </c>
       <c r="G80" t="s">
         <v>339</v>
       </c>
-      <c r="H80" t="n">
-        <v>0.5105059742927551</v>
-      </c>
-      <c r="I80" t="n">
+      <c r="H80">
+        <v>0.51050597429275513</v>
+      </c>
+      <c r="I80">
         <v>0.14066700637340546</v>
       </c>
-      <c r="J80" t="n">
-        <v>79.0</v>
+      <c r="J80">
+        <v>79</v>
       </c>
       <c r="K80" t="s">
         <v>340</v>
@@ -4818,7 +5152,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -4834,20 +5168,20 @@
       <c r="E81" t="s">
         <v>17</v>
       </c>
-      <c r="F81" t="n">
-        <v>52.0</v>
+      <c r="F81">
+        <v>52</v>
       </c>
       <c r="G81" t="s">
         <v>343</v>
       </c>
-      <c r="H81" t="n">
-        <v>0.2985360026359558</v>
-      </c>
-      <c r="I81" t="n">
+      <c r="H81">
+        <v>0.29853600263595581</v>
+      </c>
+      <c r="I81">
         <v>0.21585799753665924</v>
       </c>
-      <c r="J81" t="n">
-        <v>80.0</v>
+      <c r="J81">
+        <v>80</v>
       </c>
       <c r="K81" t="s">
         <v>344</v>
@@ -4859,7 +5193,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>13</v>
       </c>
@@ -4875,20 +5209,20 @@
       <c r="E82" t="s">
         <v>17</v>
       </c>
-      <c r="F82" t="n">
-        <v>55.0</v>
+      <c r="F82">
+        <v>55</v>
       </c>
       <c r="G82" t="s">
         <v>348</v>
       </c>
-      <c r="H82" t="n">
+      <c r="H82">
         <v>0.1931300014257431</v>
       </c>
-      <c r="I82" t="n">
-        <v>0.1719149947166443</v>
-      </c>
-      <c r="J82" t="n">
-        <v>81.0</v>
+      <c r="I82">
+        <v>0.17191499471664429</v>
+      </c>
+      <c r="J82">
+        <v>81</v>
       </c>
       <c r="K82" t="s">
         <v>349</v>
@@ -4900,7 +5234,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -4916,20 +5250,20 @@
       <c r="E83" t="s">
         <v>17</v>
       </c>
-      <c r="F83" t="n">
-        <v>55.0</v>
+      <c r="F83">
+        <v>55</v>
       </c>
       <c r="G83" t="s">
         <v>353</v>
       </c>
-      <c r="H83" t="n">
-        <v>0.3154299855232239</v>
-      </c>
-      <c r="I83" t="n">
+      <c r="H83">
+        <v>0.31542998552322388</v>
+      </c>
+      <c r="I83">
         <v>0.15526600182056427</v>
       </c>
-      <c r="J83" t="n">
-        <v>82.0</v>
+      <c r="J83">
+        <v>82</v>
       </c>
       <c r="K83" t="s">
         <v>354</v>
@@ -4941,7 +5275,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -4957,20 +5291,20 @@
       <c r="E84" t="s">
         <v>17</v>
       </c>
-      <c r="F84" t="n">
-        <v>55.0</v>
+      <c r="F84">
+        <v>55</v>
       </c>
       <c r="G84" t="s">
         <v>357</v>
       </c>
-      <c r="H84" t="n">
-        <v>0.5801010131835938</v>
-      </c>
-      <c r="I84" t="n">
-        <v>0.1213039979338646</v>
-      </c>
-      <c r="J84" t="n">
-        <v>83.0</v>
+      <c r="H84">
+        <v>0.58010101318359375</v>
+      </c>
+      <c r="I84">
+        <v>0.12130399793386459</v>
+      </c>
+      <c r="J84">
+        <v>83</v>
       </c>
       <c r="K84" t="s">
         <v>358</v>
@@ -4982,7 +5316,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -4998,20 +5332,20 @@
       <c r="E85" t="s">
         <v>17</v>
       </c>
-      <c r="F85" t="n">
-        <v>56.0</v>
+      <c r="F85">
+        <v>56</v>
       </c>
       <c r="G85" t="s">
         <v>361</v>
       </c>
-      <c r="H85" t="n">
-        <v>0.5352380275726318</v>
-      </c>
-      <c r="I85" t="n">
+      <c r="H85">
+        <v>0.53523802757263184</v>
+      </c>
+      <c r="I85">
         <v>0.13967600464820862</v>
       </c>
-      <c r="J85" t="n">
-        <v>84.0</v>
+      <c r="J85">
+        <v>84</v>
       </c>
       <c r="K85" t="s">
         <v>362</v>
@@ -5023,7 +5357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>13</v>
       </c>
@@ -5039,20 +5373,20 @@
       <c r="E86" t="s">
         <v>17</v>
       </c>
-      <c r="F86" t="n">
-        <v>58.0</v>
+      <c r="F86">
+        <v>58</v>
       </c>
       <c r="G86" t="s">
         <v>365</v>
       </c>
-      <c r="H86" t="n">
+      <c r="H86">
         <v>0.5486530065536499</v>
       </c>
-      <c r="I86" t="n">
+      <c r="I86">
         <v>0.1342799961566925</v>
       </c>
-      <c r="J86" t="n">
-        <v>85.0</v>
+      <c r="J86">
+        <v>85</v>
       </c>
       <c r="K86" t="s">
         <v>366</v>
@@ -5064,7 +5398,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>13</v>
       </c>
@@ -5080,20 +5414,20 @@
       <c r="E87" t="s">
         <v>17</v>
       </c>
-      <c r="F87" t="n">
-        <v>59.0</v>
+      <c r="F87">
+        <v>59</v>
       </c>
       <c r="G87" t="s">
         <v>370</v>
       </c>
-      <c r="H87" t="n">
-        <v>0.5421800017356873</v>
-      </c>
-      <c r="I87" t="n">
-        <v>0.108365997672081</v>
-      </c>
-      <c r="J87" t="n">
-        <v>86.0</v>
+      <c r="H87">
+        <v>0.54218000173568726</v>
+      </c>
+      <c r="I87">
+        <v>0.10836599767208099</v>
+      </c>
+      <c r="J87">
+        <v>86</v>
       </c>
       <c r="K87" t="s">
         <v>371</v>
@@ -5105,7 +5439,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>13</v>
       </c>
@@ -5121,20 +5455,20 @@
       <c r="E88" t="s">
         <v>17</v>
       </c>
-      <c r="F88" t="n">
-        <v>60.0</v>
+      <c r="F88">
+        <v>60</v>
       </c>
       <c r="G88" t="s">
         <v>375</v>
       </c>
-      <c r="H88" t="n">
+      <c r="H88">
         <v>0.43587398529052734</v>
       </c>
-      <c r="I88" t="n">
+      <c r="I88">
         <v>0.12226700037717819</v>
       </c>
-      <c r="J88" t="n">
-        <v>87.0</v>
+      <c r="J88">
+        <v>87</v>
       </c>
       <c r="K88" t="s">
         <v>376</v>
@@ -5146,7 +5480,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>13</v>
       </c>
@@ -5162,20 +5496,20 @@
       <c r="E89" t="s">
         <v>17</v>
       </c>
-      <c r="F89" t="n">
-        <v>63.0</v>
+      <c r="F89">
+        <v>63</v>
       </c>
       <c r="G89" t="s">
         <v>379</v>
       </c>
-      <c r="H89" t="n">
-        <v>0.6632450222969055</v>
-      </c>
-      <c r="I89" t="n">
-        <v>0.088189996778965</v>
-      </c>
-      <c r="J89" t="n">
-        <v>88.0</v>
+      <c r="H89">
+        <v>0.66324502229690552</v>
+      </c>
+      <c r="I89">
+        <v>8.8189996778964996E-2</v>
+      </c>
+      <c r="J89">
+        <v>88</v>
       </c>
       <c r="K89" t="s">
         <v>380</v>
@@ -5187,7 +5521,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>13</v>
       </c>
@@ -5203,20 +5537,20 @@
       <c r="E90" t="s">
         <v>17</v>
       </c>
-      <c r="F90" t="n">
-        <v>65.0</v>
+      <c r="F90">
+        <v>65</v>
       </c>
       <c r="G90" t="s">
         <v>383</v>
       </c>
-      <c r="H90" t="n">
-        <v>0.3981109857559204</v>
-      </c>
-      <c r="I90" t="n">
-        <v>0.08822160214185715</v>
-      </c>
-      <c r="J90" t="n">
-        <v>89.0</v>
+      <c r="H90">
+        <v>0.39811098575592041</v>
+      </c>
+      <c r="I90">
+        <v>8.8221602141857147E-2</v>
+      </c>
+      <c r="J90">
+        <v>89</v>
       </c>
       <c r="K90" t="s">
         <v>384</v>
@@ -5228,7 +5562,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>13</v>
       </c>
@@ -5244,20 +5578,20 @@
       <c r="E91" t="s">
         <v>17</v>
       </c>
-      <c r="F91" t="n">
-        <v>66.0</v>
+      <c r="F91">
+        <v>66</v>
       </c>
       <c r="G91" t="s">
         <v>388</v>
       </c>
-      <c r="H91" t="n">
-        <v>0.5310699939727783</v>
-      </c>
-      <c r="I91" t="n">
-        <v>0.0811987966299057</v>
-      </c>
-      <c r="J91" t="n">
-        <v>90.0</v>
+      <c r="H91">
+        <v>0.53106999397277832</v>
+      </c>
+      <c r="I91">
+        <v>8.1198796629905701E-2</v>
+      </c>
+      <c r="J91">
+        <v>90</v>
       </c>
       <c r="K91" t="s">
         <v>389</v>
@@ -5269,7 +5603,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>13</v>
       </c>
@@ -5285,20 +5619,20 @@
       <c r="E92" t="s">
         <v>17</v>
       </c>
-      <c r="F92" t="n">
-        <v>68.0</v>
+      <c r="F92">
+        <v>68</v>
       </c>
       <c r="G92" t="s">
         <v>392</v>
       </c>
-      <c r="H92" t="n">
-        <v>0.4617289900779724</v>
-      </c>
-      <c r="I92" t="n">
+      <c r="H92">
+        <v>0.46172899007797241</v>
+      </c>
+      <c r="I92">
         <v>0.12698200345039368</v>
       </c>
-      <c r="J92" t="n">
-        <v>91.0</v>
+      <c r="J92">
+        <v>91</v>
       </c>
       <c r="K92" t="s">
         <v>393</v>
@@ -5310,7 +5644,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>13</v>
       </c>
@@ -5326,20 +5660,20 @@
       <c r="E93" t="s">
         <v>17</v>
       </c>
-      <c r="F93" t="n">
-        <v>69.0</v>
+      <c r="F93">
+        <v>69</v>
       </c>
       <c r="G93" t="s">
         <v>397</v>
       </c>
-      <c r="H93" t="n">
+      <c r="H93">
         <v>0.49941501021385193</v>
       </c>
-      <c r="I93" t="n">
+      <c r="I93">
         <v>0.12094199657440186</v>
       </c>
-      <c r="J93" t="n">
-        <v>92.0</v>
+      <c r="J93">
+        <v>92</v>
       </c>
       <c r="K93" t="s">
         <v>398</v>
@@ -5351,7 +5685,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -5367,20 +5701,20 @@
       <c r="E94" t="s">
         <v>17</v>
       </c>
-      <c r="F94" t="n">
-        <v>70.0</v>
+      <c r="F94">
+        <v>70</v>
       </c>
       <c r="G94" t="s">
         <v>402</v>
       </c>
-      <c r="H94" t="n">
-        <v>0.6708359718322754</v>
-      </c>
-      <c r="I94" t="n">
+      <c r="H94">
+        <v>0.67083597183227539</v>
+      </c>
+      <c r="I94">
         <v>0.12462899833917618</v>
       </c>
-      <c r="J94" t="n">
-        <v>93.0</v>
+      <c r="J94">
+        <v>93</v>
       </c>
       <c r="K94" t="s">
         <v>403</v>
@@ -5392,7 +5726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>13</v>
       </c>
@@ -5408,20 +5742,20 @@
       <c r="E95" t="s">
         <v>17</v>
       </c>
-      <c r="F95" t="n">
-        <v>72.0</v>
+      <c r="F95">
+        <v>72</v>
       </c>
       <c r="G95" t="s">
         <v>407</v>
       </c>
-      <c r="H95" t="n">
-        <v>0.4482640027999878</v>
-      </c>
-      <c r="I95" t="n">
-        <v>0.07062090188264847</v>
-      </c>
-      <c r="J95" t="n">
-        <v>94.0</v>
+      <c r="H95">
+        <v>0.44826400279998779</v>
+      </c>
+      <c r="I95">
+        <v>7.0620901882648468E-2</v>
+      </c>
+      <c r="J95">
+        <v>94</v>
       </c>
       <c r="K95" t="s">
         <v>408</v>
@@ -5433,7 +5767,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>13</v>
       </c>
@@ -5449,20 +5783,20 @@
       <c r="E96" t="s">
         <v>17</v>
       </c>
-      <c r="F96" t="n">
-        <v>78.0</v>
+      <c r="F96">
+        <v>78</v>
       </c>
       <c r="G96" t="s">
         <v>411</v>
       </c>
-      <c r="H96" t="n">
+      <c r="H96">
         <v>0.4981440007686615</v>
       </c>
-      <c r="I96" t="n">
+      <c r="I96">
         <v>0.18422099947929382</v>
       </c>
-      <c r="J96" t="n">
-        <v>95.0</v>
+      <c r="J96">
+        <v>95</v>
       </c>
       <c r="K96" t="s">
         <v>412</v>
@@ -5474,7 +5808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>13</v>
       </c>
@@ -5490,20 +5824,20 @@
       <c r="E97" t="s">
         <v>17</v>
       </c>
-      <c r="F97" t="n">
-        <v>79.0</v>
+      <c r="F97">
+        <v>79</v>
       </c>
       <c r="G97" t="s">
         <v>416</v>
       </c>
-      <c r="H97" t="n">
+      <c r="H97">
         <v>0.3849090039730072</v>
       </c>
-      <c r="I97" t="n">
+      <c r="I97">
         <v>0.15057599544525146</v>
       </c>
-      <c r="J97" t="n">
-        <v>96.0</v>
+      <c r="J97">
+        <v>96</v>
       </c>
       <c r="K97" t="s">
         <v>417</v>
@@ -5515,7 +5849,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -5531,20 +5865,20 @@
       <c r="E98" t="s">
         <v>17</v>
       </c>
-      <c r="F98" t="n">
-        <v>80.0</v>
+      <c r="F98">
+        <v>80</v>
       </c>
       <c r="G98" t="s">
         <v>420</v>
       </c>
-      <c r="H98" t="n">
-        <v>0.4880799949169159</v>
-      </c>
-      <c r="I98" t="n">
+      <c r="H98">
+        <v>0.48807999491691589</v>
+      </c>
+      <c r="I98">
         <v>0.11850199848413467</v>
       </c>
-      <c r="J98" t="n">
-        <v>97.0</v>
+      <c r="J98">
+        <v>97</v>
       </c>
       <c r="K98" t="s">
         <v>421</v>
@@ -5556,7 +5890,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>13</v>
       </c>
@@ -5572,20 +5906,20 @@
       <c r="E99" t="s">
         <v>17</v>
       </c>
-      <c r="F99" t="n">
-        <v>81.0</v>
+      <c r="F99">
+        <v>81</v>
       </c>
       <c r="G99" t="s">
         <v>424</v>
       </c>
-      <c r="H99" t="n">
-        <v>0.5902100205421448</v>
-      </c>
-      <c r="I99" t="n">
-        <v>0.09401030093431473</v>
-      </c>
-      <c r="J99" t="n">
-        <v>98.0</v>
+      <c r="H99">
+        <v>0.59021002054214478</v>
+      </c>
+      <c r="I99">
+        <v>9.4010300934314728E-2</v>
+      </c>
+      <c r="J99">
+        <v>98</v>
       </c>
       <c r="K99" t="s">
         <v>425</v>
@@ -5597,7 +5931,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>13</v>
       </c>
@@ -5613,20 +5947,20 @@
       <c r="E100" t="s">
         <v>17</v>
       </c>
-      <c r="F100" t="n">
-        <v>87.0</v>
+      <c r="F100">
+        <v>87</v>
       </c>
       <c r="G100" t="s">
         <v>429</v>
       </c>
-      <c r="H100" t="n">
-        <v>0.5937060117721558</v>
-      </c>
-      <c r="I100" t="n">
-        <v>0.0531201995909214</v>
-      </c>
-      <c r="J100" t="n">
-        <v>99.0</v>
+      <c r="H100">
+        <v>0.59370601177215576</v>
+      </c>
+      <c r="I100">
+        <v>5.3120199590921402E-2</v>
+      </c>
+      <c r="J100">
+        <v>99</v>
       </c>
       <c r="K100" t="s">
         <v>430</v>
@@ -5638,7 +5972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>13</v>
       </c>
@@ -5654,20 +5988,20 @@
       <c r="E101" t="s">
         <v>17</v>
       </c>
-      <c r="F101" t="n">
-        <v>96.0</v>
+      <c r="F101">
+        <v>96</v>
       </c>
       <c r="G101" t="s">
         <v>433</v>
       </c>
-      <c r="H101" t="n">
-        <v>0.6456900238990784</v>
-      </c>
-      <c r="I101" t="n">
-        <v>0.09339609742164612</v>
-      </c>
-      <c r="J101" t="n">
-        <v>100.0</v>
+      <c r="H101">
+        <v>0.64569002389907837</v>
+      </c>
+      <c r="I101">
+        <v>9.3396097421646118E-2</v>
+      </c>
+      <c r="J101">
+        <v>100</v>
       </c>
       <c r="K101" t="s">
         <v>434</v>
@@ -5679,7 +6013,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>13</v>
       </c>
@@ -5695,20 +6029,20 @@
       <c r="E102" t="s">
         <v>17</v>
       </c>
-      <c r="F102" t="n">
-        <v>102.0</v>
+      <c r="F102">
+        <v>102</v>
       </c>
       <c r="G102" t="s">
         <v>437</v>
       </c>
-      <c r="H102" t="n">
-        <v>0.3279019892215729</v>
-      </c>
-      <c r="I102" t="n">
-        <v>0.08509320020675659</v>
-      </c>
-      <c r="J102" t="n">
-        <v>101.0</v>
+      <c r="H102">
+        <v>0.32790198922157288</v>
+      </c>
+      <c r="I102">
+        <v>8.5093200206756592E-2</v>
+      </c>
+      <c r="J102">
+        <v>101</v>
       </c>
       <c r="K102" t="s">
         <v>417</v>
@@ -5720,7 +6054,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>13</v>
       </c>
@@ -5736,20 +6070,20 @@
       <c r="E103" t="s">
         <v>17</v>
       </c>
-      <c r="F103" t="n">
-        <v>105.0</v>
+      <c r="F103">
+        <v>105</v>
       </c>
       <c r="G103" t="s">
         <v>441</v>
       </c>
-      <c r="H103" t="n">
+      <c r="H103">
         <v>0.30167800188064575</v>
       </c>
-      <c r="I103" t="n">
-        <v>0.09260209649801254</v>
-      </c>
-      <c r="J103" t="n">
-        <v>102.0</v>
+      <c r="I103">
+        <v>9.2602096498012543E-2</v>
+      </c>
+      <c r="J103">
+        <v>102</v>
       </c>
       <c r="K103" t="s">
         <v>442</v>
@@ -5761,7 +6095,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>13</v>
       </c>
@@ -5777,20 +6111,20 @@
       <c r="E104" t="s">
         <v>17</v>
       </c>
-      <c r="F104" t="n">
-        <v>110.0</v>
+      <c r="F104">
+        <v>110</v>
       </c>
       <c r="G104" t="s">
         <v>446</v>
       </c>
-      <c r="H104" t="n">
-        <v>0.6415359973907471</v>
-      </c>
-      <c r="I104" t="n">
-        <v>0.059972699731588364</v>
-      </c>
-      <c r="J104" t="n">
-        <v>103.0</v>
+      <c r="H104">
+        <v>0.64153599739074707</v>
+      </c>
+      <c r="I104">
+        <v>5.9972699731588364E-2</v>
+      </c>
+      <c r="J104">
+        <v>103</v>
       </c>
       <c r="K104" t="s">
         <v>447</v>
@@ -5802,7 +6136,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>13</v>
       </c>
@@ -5818,20 +6152,20 @@
       <c r="E105" t="s">
         <v>17</v>
       </c>
-      <c r="F105" t="n">
-        <v>115.0</v>
+      <c r="F105">
+        <v>115</v>
       </c>
       <c r="G105" t="s">
         <v>451</v>
       </c>
-      <c r="H105" t="n">
-        <v>0.5005139708518982</v>
-      </c>
-      <c r="I105" t="n">
-        <v>0.03676670044660568</v>
-      </c>
-      <c r="J105" t="n">
-        <v>104.0</v>
+      <c r="H105">
+        <v>0.50051397085189819</v>
+      </c>
+      <c r="I105">
+        <v>3.6766700446605682E-2</v>
+      </c>
+      <c r="J105">
+        <v>104</v>
       </c>
       <c r="K105" t="s">
         <v>452</v>
@@ -5843,7 +6177,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -5859,20 +6193,20 @@
       <c r="E106" t="s">
         <v>17</v>
       </c>
-      <c r="F106" t="n">
-        <v>116.0</v>
+      <c r="F106">
+        <v>116</v>
       </c>
       <c r="G106" t="s">
         <v>455</v>
       </c>
-      <c r="H106" t="n">
-        <v>0.5590100288391113</v>
-      </c>
-      <c r="I106" t="n">
-        <v>0.07586350291967392</v>
-      </c>
-      <c r="J106" t="n">
-        <v>105.0</v>
+      <c r="H106">
+        <v>0.55901002883911133</v>
+      </c>
+      <c r="I106">
+        <v>7.586350291967392E-2</v>
+      </c>
+      <c r="J106">
+        <v>105</v>
       </c>
       <c r="K106" t="s">
         <v>456</v>
@@ -5884,7 +6218,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -5900,20 +6234,20 @@
       <c r="E107" t="s">
         <v>17</v>
       </c>
-      <c r="F107" t="n">
-        <v>121.0</v>
+      <c r="F107">
+        <v>121</v>
       </c>
       <c r="G107" t="s">
         <v>460</v>
       </c>
-      <c r="H107" t="n">
-        <v>0.5875459909439087</v>
-      </c>
-      <c r="I107" t="n">
+      <c r="H107">
+        <v>0.58754599094390869</v>
+      </c>
+      <c r="I107">
         <v>0.11747600138187408</v>
       </c>
-      <c r="J107" t="n">
-        <v>106.0</v>
+      <c r="J107">
+        <v>106</v>
       </c>
       <c r="K107" t="s">
         <v>461</v>
@@ -5925,7 +6259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>13</v>
       </c>
@@ -5941,20 +6275,20 @@
       <c r="E108" t="s">
         <v>17</v>
       </c>
-      <c r="F108" t="n">
-        <v>130.0</v>
+      <c r="F108">
+        <v>130</v>
       </c>
       <c r="G108" t="s">
         <v>464</v>
       </c>
-      <c r="H108" t="n">
-        <v>0.5213080048561096</v>
-      </c>
-      <c r="I108" t="n">
-        <v>0.07781500369310379</v>
-      </c>
-      <c r="J108" t="n">
-        <v>107.0</v>
+      <c r="H108">
+        <v>0.52130800485610962</v>
+      </c>
+      <c r="I108">
+        <v>7.781500369310379E-2</v>
+      </c>
+      <c r="J108">
+        <v>107</v>
       </c>
       <c r="K108" t="s">
         <v>465</v>
@@ -5966,7 +6300,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>13</v>
       </c>
@@ -5982,20 +6316,20 @@
       <c r="E109" t="s">
         <v>17</v>
       </c>
-      <c r="F109" t="n">
-        <v>133.0</v>
+      <c r="F109">
+        <v>133</v>
       </c>
       <c r="G109" t="s">
         <v>469</v>
       </c>
-      <c r="H109" t="n">
-        <v>0.6407099962234497</v>
-      </c>
-      <c r="I109" t="n">
-        <v>0.03726070001721382</v>
-      </c>
-      <c r="J109" t="n">
-        <v>108.0</v>
+      <c r="H109">
+        <v>0.64070999622344971</v>
+      </c>
+      <c r="I109">
+        <v>3.7260700017213821E-2</v>
+      </c>
+      <c r="J109">
+        <v>108</v>
       </c>
       <c r="K109" t="s">
         <v>470</v>
@@ -6007,7 +6341,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>13</v>
       </c>
@@ -6023,20 +6357,20 @@
       <c r="E110" t="s">
         <v>17</v>
       </c>
-      <c r="F110" t="n">
-        <v>192.0</v>
+      <c r="F110">
+        <v>192</v>
       </c>
       <c r="G110" t="s">
         <v>473</v>
       </c>
-      <c r="H110" t="n">
+      <c r="H110">
         <v>0.44971200823783875</v>
       </c>
-      <c r="I110" t="n">
-        <v>0.030359700322151184</v>
-      </c>
-      <c r="J110" t="n">
-        <v>109.0</v>
+      <c r="I110">
+        <v>3.0359700322151184E-2</v>
+      </c>
+      <c r="J110">
+        <v>109</v>
       </c>
       <c r="K110" t="s">
         <v>474</v>
@@ -6048,7 +6382,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>13</v>
       </c>
@@ -6064,20 +6398,20 @@
       <c r="E111" t="s">
         <v>17</v>
       </c>
-      <c r="F111" t="n">
-        <v>205.0</v>
+      <c r="F111">
+        <v>205</v>
       </c>
       <c r="G111" t="s">
         <v>477</v>
       </c>
-      <c r="H111" t="n">
-        <v>0.5484610199928284</v>
-      </c>
-      <c r="I111" t="n">
-        <v>0.04849030077457428</v>
-      </c>
-      <c r="J111" t="n">
-        <v>110.0</v>
+      <c r="H111">
+        <v>0.54846101999282837</v>
+      </c>
+      <c r="I111">
+        <v>4.849030077457428E-2</v>
+      </c>
+      <c r="J111">
+        <v>110</v>
       </c>
       <c r="K111" t="s">
         <v>478</v>
@@ -6089,7 +6423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>13</v>
       </c>
@@ -6105,20 +6439,20 @@
       <c r="E112" t="s">
         <v>17</v>
       </c>
-      <c r="F112" t="n">
-        <v>259.0</v>
+      <c r="F112">
+        <v>259</v>
       </c>
       <c r="G112" t="s">
         <v>481</v>
       </c>
-      <c r="H112" t="n">
-        <v>0.4779900014400482</v>
-      </c>
-      <c r="I112" t="n">
-        <v>0.03250949829816818</v>
-      </c>
-      <c r="J112" t="n">
-        <v>111.0</v>
+      <c r="H112">
+        <v>0.47799000144004822</v>
+      </c>
+      <c r="I112">
+        <v>3.2509498298168182E-2</v>
+      </c>
+      <c r="J112">
+        <v>111</v>
       </c>
       <c r="K112" t="s">
         <v>482</v>
@@ -6130,7 +6464,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>13</v>
       </c>
@@ -6146,20 +6480,20 @@
       <c r="E113" t="s">
         <v>17</v>
       </c>
-      <c r="F113" t="n">
-        <v>285.0</v>
+      <c r="F113">
+        <v>285</v>
       </c>
       <c r="G113" t="s">
         <v>485</v>
       </c>
-      <c r="H113" t="n">
+      <c r="H113">
         <v>0.4568139910697937</v>
       </c>
-      <c r="I113" t="n">
-        <v>0.0496021993458271</v>
-      </c>
-      <c r="J113" t="n">
-        <v>112.0</v>
+      <c r="I113">
+        <v>4.9602199345827103E-2</v>
+      </c>
+      <c r="J113">
+        <v>112</v>
       </c>
       <c r="K113" t="s">
         <v>486</v>
@@ -6171,7 +6505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>13</v>
       </c>
@@ -6187,20 +6521,20 @@
       <c r="E114" t="s">
         <v>17</v>
       </c>
-      <c r="F114" t="n">
-        <v>905.0</v>
+      <c r="F114">
+        <v>905</v>
       </c>
       <c r="G114" t="s">
         <v>490</v>
       </c>
-      <c r="H114" t="n">
+      <c r="H114">
         <v>0.6748809814453125</v>
       </c>
-      <c r="I114" t="n">
-        <v>0.05451580137014389</v>
-      </c>
-      <c r="J114" t="n">
-        <v>113.0</v>
+      <c r="I114">
+        <v>5.451580137014389E-2</v>
+      </c>
+      <c r="J114">
+        <v>113</v>
       </c>
       <c r="K114" t="s">
         <v>491</v>
@@ -6213,6 +6547,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>